<commit_message>
Schematic done. PCB layout started
</commit_message>
<xml_diff>
--- a/Hardware/Calcs.xlsx
+++ b/Hardware/Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago Silva\Documents\Eagle\projects\PowerSpy\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C623BEB-32B1-4A26-9303-F632BEEE74EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDCDB56-0DA6-4B9F-947C-8572361EA086}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4245" windowWidth="28800" windowHeight="11505" xr2:uid="{FF9F9078-04B1-4408-B7C9-7B1BBA45B5CE}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="4245" windowWidth="28800" windowHeight="11505" xr2:uid="{FF9F9078-04B1-4408-B7C9-7B1BBA45B5CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>VRMS</t>
   </si>
@@ -78,9 +78,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>PMÁX</t>
-  </si>
-  <si>
     <t>https://www.eletrodex.com.br/mfpt-conector-mini-fit-4-2mm-90-metaltex.html</t>
   </si>
   <si>
@@ -91,15 +88,31 @@
   </si>
   <si>
     <t>https://www.eletrodex.com.br/led-smd-5050-rgb-difuso-120.html</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>PMÁX [W]</t>
+  </si>
+  <si>
+    <t>mW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -151,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -168,6 +181,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -483,16 +501,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AF3731-A7C2-4938-AC51-C2F0192EAF79}">
-  <dimension ref="C4:K26"/>
+  <dimension ref="C4:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="8" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11.5703125" style="1" customWidth="1"/>
@@ -562,14 +580,17 @@
         <v>3</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <f>D7/D8</f>
         <v>5.0744012378441789E-4</v>
       </c>
@@ -583,6 +604,10 @@
         <f>H9*($D$9^2)</f>
         <v>5.6649005429795979E-2</v>
       </c>
+      <c r="J9" s="11">
+        <f>I9*1000</f>
+        <v>56.649005429795977</v>
+      </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H10" s="1">
@@ -592,6 +617,10 @@
         <f t="shared" ref="I10:I13" si="0">H10*($D$9^2)</f>
         <v>5.6649005429795979E-2</v>
       </c>
+      <c r="J10" s="11">
+        <f t="shared" ref="J10:J13" si="1">I10*1000</f>
+        <v>56.649005429795977</v>
+      </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H11" s="1">
@@ -601,6 +630,10 @@
         <f t="shared" si="0"/>
         <v>2.5749547922634536E-2</v>
       </c>
+      <c r="J11" s="11">
+        <f t="shared" si="1"/>
+        <v>25.749547922634537</v>
+      </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H12" s="1">
@@ -610,6 +643,10 @@
         <f t="shared" si="0"/>
         <v>2.5749547922634536E-2</v>
       </c>
+      <c r="J12" s="11">
+        <f t="shared" si="1"/>
+        <v>25.749547922634537</v>
+      </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H13" s="1">
@@ -618,6 +655,10 @@
       <c r="I13" s="7">
         <f t="shared" si="0"/>
         <v>2.5749547922634535E-4</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="1"/>
+        <v>0.25749547922634536</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
@@ -626,7 +667,7 @@
         <v>641000</v>
       </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
       <c r="H17" s="1" t="s">
         <v>7</v>
       </c>
@@ -635,7 +676,7 @@
         <v>325.26911934581187</v>
       </c>
     </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
       <c r="H18" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,7 +685,7 @@
         <v>640000</v>
       </c>
     </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:16" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
@@ -653,7 +694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>12</v>
       </c>
@@ -662,24 +703,80 @@
         <v>0.50744012378441794</v>
       </c>
     </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G23" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G24" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="9" t="s">
+    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G25" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="9" t="s">
+    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G26" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="9" t="s">
+    <row r="32" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="L32" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="N32" s="1">
+        <f>3.3-M32</f>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="O32" s="1">
+        <f>N32/0.01</f>
+        <v>149.99999999999997</v>
+      </c>
+      <c r="P32" s="1">
+        <f>O32*(0.01^2)</f>
+        <v>1.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" ref="N33:N34" si="2">3.3-M33</f>
+        <v>0.5</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" ref="O33:O34" si="3">N33/0.01</f>
+        <v>50</v>
+      </c>
+      <c r="P33" s="1">
+        <f>O33*(0.01^2)</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="O34" s="1">
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calcs and values updated for the new AFE approach
</commit_message>
<xml_diff>
--- a/Hardware/Calcs.xlsx
+++ b/Hardware/Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago Silva\Documents\Eagle\projects\PowerSpy\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE33721-C3FE-4787-AB31-21C3C2CAB914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEE0706-7500-48D0-AF00-C2A99FEE0414}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{BE46D4BC-C98C-4CF6-ABA9-D1104B6B5519}"/>
+    <workbookView xWindow="-9165" yWindow="3195" windowWidth="19200" windowHeight="10665" xr2:uid="{BE46D4BC-C98C-4CF6-ABA9-D1104B6B5519}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Vrms</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>+setpoint --&gt;</t>
+  </si>
+  <si>
+    <t>Amp. Op. Gain</t>
   </si>
 </sst>
 </file>
@@ -511,15 +514,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E903083D-FA5D-4E39-BFC6-0A0AEC8DC0D1}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -585,13 +589,14 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3.3</v>
+        <v>1.6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>3.3</v>
+        <f>C4</f>
+        <v>1.6</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -608,103 +613,116 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J6" s="4">
         <f>1/8*1000</f>
         <v>125</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
-        <f>($C$4/($C$3+$C$4))*C2</f>
-        <v>0.92133826207145053</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" s="8">
+        <f>(($C$4/($C$3+$C$4))*C2)*2</f>
+        <v>0.89578614674006518</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8">
-        <f>($C$4/($C$3+$C$4))*E2</f>
-        <v>1.5960190366592057</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E7" s="8">
+        <f>(($C$4/($C$3+$C$4))*E2)*2</f>
+        <v>1.5517555297859398</v>
+      </c>
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J7" s="6">
         <f>1/16*1000</f>
         <v>62.5</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12">
-        <f>(3.3/2)+C6</f>
-        <v>2.5713382620714507</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" s="12">
+        <f>(3.3/2)+C7</f>
+        <v>2.5457861467400651</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="13">
-        <f>(3.3/2)+E6</f>
-        <v>3.2460190366592059</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E8" s="13">
+        <f>(3.3/2)+E7</f>
+        <v>3.2017555297859399</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <f>C2/(($C$3+$C$4)*1000)</f>
-        <v>2.791934127489244E-4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <f>E2/(($C$3+$C$4)*1000)</f>
-        <v>4.8364213232097146E-4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>C2/(($C$3+$C$4)*1000)</f>
+        <v>2.7993317085627038E-4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f>E2/(($C$3+$C$4)*1000)</f>
+        <v>4.8492360305810617E-4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9">
-        <f>((220*1000)*(C8^2))*1000</f>
-        <v>17.148771578926077</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" s="9">
+        <f>((220*1000)*(C9^2))*1000</f>
+        <v>17.239767632042092</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="9">
-        <f>((220*1000)*(E8^2))*1000</f>
-        <v>51.460136674314732</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E10" s="9">
+        <f>((220*1000)*(E9^2))*1000</f>
+        <v>51.733198176628264</v>
+      </c>
+      <c r="F10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another new and better AFE approach
</commit_message>
<xml_diff>
--- a/Hardware/Calcs.xlsx
+++ b/Hardware/Calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago Silva\Documents\Eagle\projects\PowerSpy\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\Documents\Eagle\projects\PowerSpy\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEE0706-7500-48D0-AF00-C2A99FEE0414}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1248CE0E-1AFB-4CCE-A7DC-46C2174F73CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9165" yWindow="3195" windowWidth="19200" windowHeight="10665" xr2:uid="{BE46D4BC-C98C-4CF6-ABA9-D1104B6B5519}"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="28800" windowHeight="11385" xr2:uid="{BE46D4BC-C98C-4CF6-ABA9-D1104B6B5519}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,28 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
-  <si>
-    <t>Vrms</t>
-  </si>
-  <si>
-    <t>Vp</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Vout</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <r>
       <t>k</t>
@@ -74,12 +53,6 @@
     <t>mW</t>
   </si>
   <si>
-    <t>Vac</t>
-  </si>
-  <si>
-    <t>Vdc</t>
-  </si>
-  <si>
     <t>1/8</t>
   </si>
   <si>
@@ -89,17 +62,242 @@
     <t>1/4</t>
   </si>
   <si>
-    <t>+setpoint --&gt;</t>
-  </si>
-  <si>
     <t>Amp. Op. Gain</t>
+  </si>
+  <si>
+    <t>Amp. Op. VCC</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Signals Setpoint</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DIVIDER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P-OUT.OP.AMP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OUT-DIVIDER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RMS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DIVIDER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DIVIDER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RES-DIVIDER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DC</t>
+    </r>
+  </si>
+  <si>
+    <t>VOLTAGE MEASSUREMENT</t>
+  </si>
+  <si>
+    <t>CURRENT MEASSUREMENT</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CT-IN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CT-OUT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BURDEN</t>
+    </r>
+  </si>
+  <si>
+    <t>Ω</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CT-OUT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +311,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +376,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -189,17 +414,35 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,219 +757,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E903083D-FA5D-4E39-BFC6-0A0AEC8DC0D1}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2">
+        <v>220</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9">
+        <f>B2*SQRT(2)</f>
+        <v>179.60512242138307</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="12">
+        <f>D2*SQRT(2)</f>
+        <v>311.12698372208092</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f>200+200+200</f>
+        <v>600</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>127</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2">
-        <v>220</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11">
-        <f>C1*SQRT(2)</f>
-        <v>179.60512242138307</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="14">
-        <f>E1*SQRT(2)</f>
-        <v>311.12698372208092</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f>220+220+100+100</f>
-        <v>640</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D5">
+        <f>B5</f>
+        <v>600</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>B6</f>
+        <v>1.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7">
+        <f>(($B$6/($B$5+$B$6))*B3)*2</f>
+        <v>0.89578614674006518</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7">
+        <f>(($B$6/($B$5+$B$6))*D3)*2</f>
+        <v>1.5517555297859398</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <f>220+220+100+100</f>
-        <v>640</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1.6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <f>C4</f>
-        <v>1.6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="B9" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7">
+        <f>B9</f>
+        <v>3.3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="17">
         <f>1/4*1000</f>
         <v>250</v>
       </c>
-      <c r="K4" t="s">
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="B10">
+        <f>B9/2</f>
+        <v>1.65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <f>B10</f>
+        <v>1.65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="17">
         <f>1/8*1000</f>
         <v>125</v>
       </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f>B11</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
-        <f>(($C$4/($C$3+$C$4))*C2)*2</f>
-        <v>0.89578614674006518</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8">
-        <f>(($C$4/($C$3+$C$4))*E2)*2</f>
-        <v>1.5517555297859398</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="H11" s="18">
         <f>1/16*1000</f>
         <v>62.5</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="I11" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <f>B7+B10</f>
+        <v>2.5457861467400651</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="11">
+        <f>D7+B10</f>
+        <v>3.2017555297859399</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B3/(($B$5+$B$6)*1000)</f>
+        <v>2.9859538224668837E-4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>D3/(($B$5+$B$6)*1000)</f>
+        <v>5.1725184326197992E-4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="8">
+        <f>((200*1000)*(B14^2))*1000</f>
+        <v>17.83184045980919</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <f>((200*1000)*(D14^2))*1000</f>
+        <v>53.509893871583166</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>0.05</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>33</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f>B19*B20</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B24">
+        <f>B23/2</f>
+        <v>1.65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C8" s="12">
-        <f>(3.3/2)+C7</f>
-        <v>2.5457861467400651</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="13">
-        <f>(3.3/2)+E7</f>
-        <v>3.2017555297859399</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <f>C2/(($C$3+$C$4)*1000)</f>
-        <v>2.7993317085627038E-4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <f>E2/(($C$3+$C$4)*1000)</f>
-        <v>4.8492360305810617E-4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9">
-        <f>((220*1000)*(C9^2))*1000</f>
-        <v>17.239767632042092</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="9">
-        <f>((220*1000)*(E9^2))*1000</f>
-        <v>51.733198176628264</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
+      <c r="B26" s="20">
+        <f>B21+B24</f>
+        <v>3.3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Pull-down resistor added to current AFE
</commit_message>
<xml_diff>
--- a/Hardware/Calcs.xlsx
+++ b/Hardware/Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\Documents\Eagle\projects\PowerSpy\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1248CE0E-1AFB-4CCE-A7DC-46C2174F73CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AAE8A5-E488-4DED-B719-751FA774978E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2850" windowWidth="28800" windowHeight="11385" xr2:uid="{BE46D4BC-C98C-4CF6-ABA9-D1104B6B5519}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <r>
       <t>k</t>
@@ -291,6 +291,9 @@
       </rPr>
       <t>CT-OUT</t>
     </r>
+  </si>
+  <si>
+    <t>Amp. Op. VDD</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -760,7 +763,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,13 +776,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -870,7 +873,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="7">
-        <f>(($B$6/($B$5+$B$6))*D3)*2</f>
+        <f>(($D$6/($D$5+$D$6))*D3)*2</f>
         <v>1.5517555297859398</v>
       </c>
       <c r="E7" t="s">
@@ -885,7 +888,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B9" s="7">
         <v>3.3</v>
@@ -974,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="11">
-        <f>D7+B10</f>
+        <f>D7+D10</f>
         <v>3.2017555297859399</v>
       </c>
       <c r="E12" t="s">
@@ -1023,13 +1026,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">

</xml_diff>